<commit_message>
researc h         down llapod upadfteaw
</commit_message>
<xml_diff>
--- a/form1_responses.xlsx
+++ b/form1_responses.xlsx
@@ -434,7 +434,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Emerging Technology Course-I, Communicative English</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>